<commit_message>
minor revisions from Dec2018
</commit_message>
<xml_diff>
--- a/Jan_2019.xlsx
+++ b/Jan_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohdasti/Documents/GitHub/Queens-Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181EEC85-54BE-9A40-9716-06138694EACD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DC6502-F220-F342-B7C4-7095F80F2837}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{0C37DF05-7FDA-B342-9691-799E7F642A94}"/>
   </bookViews>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="173">
   <si>
     <t>Date</t>
   </si>
@@ -682,9 +682,6 @@
   </si>
   <si>
     <t>MC3</t>
-  </si>
-  <si>
-    <t>November 13,2018</t>
   </si>
   <si>
     <t>breathing and thinking of white space</t>
@@ -745,12 +742,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="yyyy/mm/dd;@"/>
-    <numFmt numFmtId="168" formatCode="[$-1009]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="169" formatCode="hh:mm:ss;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
@@ -1085,21 +1081,6 @@
     <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1112,6 +1093,21 @@
     <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1428,9 +1424,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EEF925-A145-1E4C-BE46-D057DDAEEF7F}">
   <dimension ref="A1:GQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR1" sqref="AR1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1614,7 +1610,7 @@
         <v>140</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AW1" s="2" t="s">
         <v>26</v>
@@ -1635,10 +1631,10 @@
         <v>151</v>
       </c>
       <c r="BC1" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="BD1" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="BD1" s="8" t="s">
-        <v>172</v>
       </c>
       <c r="BE1" s="8" t="s">
         <v>38</v>
@@ -1679,13 +1675,13 @@
       <c r="A2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="88">
+      <c r="B2" s="96">
         <v>43052</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="95">
+      <c r="D2" s="90">
         <v>0.4375</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -1877,13 +1873,13 @@
       <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="88">
+      <c r="B3" s="96">
         <v>43065</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="95">
+      <c r="D3" s="90">
         <v>0.52083333333333337</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -2077,13 +2073,13 @@
       <c r="A4" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="88">
+      <c r="B4" s="96">
         <v>43069</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="95">
+      <c r="D4" s="90">
         <v>0.47916666666666669</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -2275,13 +2271,13 @@
       <c r="A5" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="88">
+      <c r="B5" s="96">
         <v>43073</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="95">
+      <c r="D5" s="90">
         <v>0.45833333333333331</v>
       </c>
       <c r="E5" s="10" t="s">
@@ -2473,13 +2469,13 @@
       <c r="A6" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="88">
+      <c r="B6" s="96">
         <v>43079</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="95">
+      <c r="D6" s="90">
         <v>0.5</v>
       </c>
       <c r="E6" s="18" t="s">
@@ -2671,13 +2667,13 @@
       <c r="A7" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="88">
+      <c r="B7" s="96">
         <v>43128</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="95">
+      <c r="D7" s="90">
         <v>0.5</v>
       </c>
       <c r="E7" s="18" t="s">
@@ -2875,13 +2871,13 @@
       <c r="A8" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="88">
+      <c r="B8" s="96">
         <v>43138</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="95">
+      <c r="D8" s="90">
         <v>0.47916666666666669</v>
       </c>
       <c r="E8" s="18" t="s">
@@ -3075,13 +3071,13 @@
       <c r="A9" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="88">
+      <c r="B9" s="96">
         <v>43145</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="95">
+      <c r="D9" s="90">
         <v>0.5625</v>
       </c>
       <c r="E9" s="18" t="s">
@@ -3275,13 +3271,13 @@
       <c r="A10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="88">
+      <c r="B10" s="96">
         <v>43166</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="95">
+      <c r="D10" s="90">
         <v>0.625</v>
       </c>
       <c r="E10" s="18" t="s">
@@ -3475,13 +3471,13 @@
       <c r="A11" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="88">
+      <c r="B11" s="96">
         <v>43138</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="95">
+      <c r="D11" s="90">
         <v>0.625</v>
       </c>
       <c r="E11" s="10" t="s">
@@ -3675,13 +3671,13 @@
       <c r="A12" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="88">
+      <c r="B12" s="96">
         <v>43147</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="95">
+      <c r="D12" s="90">
         <v>0.625</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -3875,13 +3871,13 @@
       <c r="A13" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="88">
+      <c r="B13" s="96">
         <v>43158</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="95">
+      <c r="D13" s="90">
         <v>0.6875</v>
       </c>
       <c r="E13" s="10" t="s">
@@ -4078,13 +4074,13 @@
       <c r="A14" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="88">
+      <c r="B14" s="96">
         <v>43168</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="95">
+      <c r="D14" s="90">
         <v>0.66666666666666663</v>
       </c>
       <c r="E14" s="10" t="s">
@@ -4281,13 +4277,13 @@
       <c r="A15" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="88">
+      <c r="B15" s="96">
         <v>43252</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="95">
+      <c r="D15" s="90">
         <v>0.6875</v>
       </c>
       <c r="E15" s="10" t="s">
@@ -4482,13 +4478,13 @@
       <c r="A16" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="88">
+      <c r="B16" s="96">
         <v>43251</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="95">
+      <c r="D16" s="90">
         <v>0.66666666666666663</v>
       </c>
       <c r="E16" s="10" t="s">
@@ -4685,13 +4681,13 @@
       <c r="A17" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="88">
+      <c r="B17" s="96">
         <v>43376</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="95">
+      <c r="D17" s="90">
         <v>0.625</v>
       </c>
       <c r="E17" s="14" t="s">
@@ -4886,13 +4882,13 @@
       <c r="A18" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="89">
+      <c r="B18" s="97">
         <v>43059</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="96">
+      <c r="D18" s="91">
         <v>0.4375</v>
       </c>
       <c r="E18" s="22" t="s">
@@ -5094,13 +5090,13 @@
       <c r="A19" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="90">
+      <c r="B19" s="98">
         <v>43124</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="97">
+      <c r="D19" s="92">
         <v>0.45833333333333331</v>
       </c>
       <c r="E19" s="34" t="s">
@@ -5302,13 +5298,13 @@
       <c r="A20" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="89">
+      <c r="B20" s="97">
         <v>43127</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="96">
+      <c r="D20" s="91">
         <v>0.5</v>
       </c>
       <c r="E20" s="22" t="s">
@@ -5516,13 +5512,13 @@
       <c r="A21" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="89">
+      <c r="B21" s="97">
         <v>43134</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="96">
+      <c r="D21" s="91">
         <v>0.58333333333333337</v>
       </c>
       <c r="E21" s="22" t="s">
@@ -5728,13 +5724,13 @@
       <c r="A22" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="89">
+      <c r="B22" s="97">
         <v>43136</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="96">
+      <c r="D22" s="91">
         <v>0.41666666666666669</v>
       </c>
       <c r="E22" s="22" t="s">
@@ -5942,13 +5938,13 @@
       <c r="A23" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="89">
+      <c r="B23" s="97">
         <v>43054</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="96">
+      <c r="D23" s="91">
         <v>0.6875</v>
       </c>
       <c r="E23" s="21" t="s">
@@ -6150,13 +6146,13 @@
       <c r="A24" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="89">
+      <c r="B24" s="97">
         <v>43061</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="96">
+      <c r="D24" s="91">
         <v>0.66666666666666663</v>
       </c>
       <c r="E24" s="21" t="s">
@@ -6364,13 +6360,13 @@
       <c r="A25" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="89">
+      <c r="B25" s="97">
         <v>43070</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="96">
+      <c r="D25" s="91">
         <v>0.60416666666666663</v>
       </c>
       <c r="E25" s="28" t="s">
@@ -6578,13 +6574,13 @@
       <c r="A26" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="91">
+      <c r="B26" s="99">
         <v>43272</v>
       </c>
       <c r="C26" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="98">
+      <c r="D26" s="93">
         <v>0.58333333333333337</v>
       </c>
       <c r="E26" s="24" t="s">
@@ -6781,13 +6777,13 @@
       <c r="A27" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="91">
+      <c r="B27" s="99">
         <v>43255</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="98">
+      <c r="D27" s="93">
         <v>0.625</v>
       </c>
       <c r="E27" s="24" t="s">
@@ -6984,13 +6980,13 @@
       <c r="A28" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="91">
+      <c r="B28" s="99">
         <v>43269</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="96">
+      <c r="D28" s="91">
         <v>0.60416666666666663</v>
       </c>
       <c r="E28" s="24" t="s">
@@ -7187,13 +7183,13 @@
       <c r="A29" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="91">
+      <c r="B29" s="99">
         <v>43262</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="98">
+      <c r="D29" s="93">
         <v>0.58333333333333337</v>
       </c>
       <c r="E29" s="24" t="s">
@@ -7390,13 +7386,13 @@
       <c r="A30" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="91">
+      <c r="B30" s="99">
         <v>43264</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="98">
+      <c r="D30" s="93">
         <v>0.58333333333333337</v>
       </c>
       <c r="E30" s="24" t="s">
@@ -7725,13 +7721,13 @@
       <c r="A31" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B31" s="91">
+      <c r="B31" s="99">
         <v>43367</v>
       </c>
       <c r="C31" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="98">
+      <c r="D31" s="93">
         <v>4.666666666666667</v>
       </c>
       <c r="E31" s="24" t="s">
@@ -8064,13 +8060,13 @@
       <c r="A32" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="B32" s="91">
+      <c r="B32" s="99">
         <v>43388</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="98">
+      <c r="D32" s="93">
         <v>0.625</v>
       </c>
       <c r="E32" s="24" t="s">
@@ -8401,13 +8397,13 @@
       <c r="A33" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B33" s="91">
+      <c r="B33" s="99">
         <v>43424</v>
       </c>
       <c r="C33" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="98">
+      <c r="D33" s="93">
         <v>0.625</v>
       </c>
       <c r="E33" s="24" t="s">
@@ -8740,13 +8736,13 @@
       <c r="A34" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="B34" s="92">
+      <c r="B34" s="100">
         <v>43062</v>
       </c>
       <c r="C34" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="99">
+      <c r="D34" s="94">
         <v>0.6875</v>
       </c>
       <c r="E34" s="43" t="s">
@@ -8938,13 +8934,13 @@
       <c r="A35" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="B35" s="92">
+      <c r="B35" s="100">
         <v>43080</v>
       </c>
       <c r="C35" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="99">
+      <c r="D35" s="94">
         <v>0.45833333333333331</v>
       </c>
       <c r="E35" s="43" t="s">
@@ -9136,13 +9132,13 @@
       <c r="A36" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="92">
+      <c r="B36" s="100">
         <v>43130</v>
       </c>
       <c r="C36" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="99">
+      <c r="D36" s="94">
         <v>0.75</v>
       </c>
       <c r="E36" s="43" t="s">
@@ -9336,13 +9332,13 @@
       <c r="A37" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="92">
+      <c r="B37" s="100">
         <v>43133</v>
       </c>
       <c r="C37" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="99">
+      <c r="D37" s="94">
         <v>0.5</v>
       </c>
       <c r="E37" s="43" t="s">
@@ -9536,13 +9532,13 @@
       <c r="A38" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="92">
+      <c r="B38" s="100">
         <v>43136</v>
       </c>
       <c r="C38" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D38" s="99">
+      <c r="D38" s="94">
         <v>0.54166666666666663</v>
       </c>
       <c r="E38" s="43" t="s">
@@ -9732,13 +9728,13 @@
       <c r="A39" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="B39" s="92">
+      <c r="B39" s="100">
         <v>43138</v>
       </c>
       <c r="C39" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="99">
+      <c r="D39" s="94">
         <v>0.35416666666666669</v>
       </c>
       <c r="E39" s="43" t="s">
@@ -9937,13 +9933,13 @@
       <c r="A40" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="B40" s="92">
+      <c r="B40" s="100">
         <v>43139</v>
       </c>
       <c r="C40" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D40" s="99">
+      <c r="D40" s="94">
         <v>0.47916666666666669</v>
       </c>
       <c r="E40" s="43" t="s">
@@ -10140,13 +10136,13 @@
       <c r="A41" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="92">
+      <c r="B41" s="100">
         <v>43145</v>
       </c>
       <c r="C41" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D41" s="99">
+      <c r="D41" s="94">
         <v>0.5</v>
       </c>
       <c r="E41" s="43" t="s">
@@ -10340,13 +10336,13 @@
       <c r="A42" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="92">
+      <c r="B42" s="100">
         <v>43132</v>
       </c>
       <c r="C42" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D42" s="99">
+      <c r="D42" s="94">
         <v>0.75</v>
       </c>
       <c r="E42" s="42" t="s">
@@ -10540,13 +10536,13 @@
       <c r="A43" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="B43" s="92">
+      <c r="B43" s="100">
         <v>43145</v>
       </c>
       <c r="C43" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D43" s="99">
+      <c r="D43" s="94">
         <v>0.625</v>
       </c>
       <c r="E43" s="42" t="s">
@@ -10742,13 +10738,13 @@
       <c r="A44" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="B44" s="92" t="s">
-        <v>155</v>
+      <c r="B44" s="100">
+        <v>43417</v>
       </c>
       <c r="C44" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="D44" s="99">
+      <c r="D44" s="94">
         <v>0.625</v>
       </c>
       <c r="E44" s="45" t="s">
@@ -10942,20 +10938,20 @@
         <v>12</v>
       </c>
       <c r="BO44" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:199" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="77" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" s="88" t="s">
         <v>157</v>
-      </c>
-      <c r="B45" s="93" t="s">
-        <v>158</v>
       </c>
       <c r="C45" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="D45" s="100">
+      <c r="D45" s="95">
         <v>0.47916666666666669</v>
       </c>
       <c r="E45" s="77" t="s">
@@ -11143,7 +11139,7 @@
         <v>53</v>
       </c>
       <c r="BM45" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BN45" s="77" t="s">
         <v>53</v>
@@ -11154,15 +11150,15 @@
     </row>
     <row r="46" spans="1:199" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" s="88" t="s">
         <v>160</v>
-      </c>
-      <c r="B46" s="93" t="s">
-        <v>161</v>
       </c>
       <c r="C46" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="D46" s="100">
+      <c r="D46" s="95">
         <v>0.41666666666666669</v>
       </c>
       <c r="E46" s="77" t="s">
@@ -11344,13 +11340,13 @@
         <v>56</v>
       </c>
       <c r="BK46" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BL46" s="86" t="s">
         <v>53</v>
       </c>
       <c r="BM46" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BN46" s="77" t="s">
         <v>53</v>
@@ -11361,15 +11357,15 @@
     </row>
     <row r="47" spans="1:199" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="77" t="s">
-        <v>162</v>
-      </c>
-      <c r="B47" s="93" t="s">
-        <v>167</v>
+        <v>161</v>
+      </c>
+      <c r="B47" s="88" t="s">
+        <v>166</v>
       </c>
       <c r="C47" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="D47" s="100">
+      <c r="D47" s="95">
         <v>0.41666666666666669</v>
       </c>
       <c r="E47" s="77" t="s">
@@ -11551,13 +11547,13 @@
         <v>63</v>
       </c>
       <c r="BK47" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BL47" s="86" t="s">
         <v>53</v>
       </c>
       <c r="BM47" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BN47" s="77" t="s">
         <v>53</v>
@@ -11568,15 +11564,15 @@
     </row>
     <row r="48" spans="1:199" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="77" t="s">
-        <v>163</v>
-      </c>
-      <c r="B48" s="93" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="B48" s="88" t="s">
+        <v>167</v>
       </c>
       <c r="C48" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="D48" s="100">
+      <c r="D48" s="95">
         <v>0.41666666666666669</v>
       </c>
       <c r="E48" s="77" t="s">
@@ -11764,7 +11760,7 @@
         <v>53</v>
       </c>
       <c r="BM48" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BN48" s="77" t="s">
         <v>53</v>
@@ -11775,15 +11771,15 @@
     </row>
     <row r="49" spans="1:67" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="77" t="s">
-        <v>164</v>
-      </c>
-      <c r="B49" s="93" t="s">
-        <v>167</v>
+        <v>163</v>
+      </c>
+      <c r="B49" s="88" t="s">
+        <v>166</v>
       </c>
       <c r="C49" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="100">
+      <c r="D49" s="95">
         <v>0.58333333333333337</v>
       </c>
       <c r="E49" s="77" t="s">
@@ -11971,7 +11967,7 @@
         <v>53</v>
       </c>
       <c r="BM49" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BN49" s="77" t="s">
         <v>53</v>
@@ -11982,15 +11978,15 @@
     </row>
     <row r="50" spans="1:67" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="77" t="s">
-        <v>165</v>
-      </c>
-      <c r="B50" s="93" t="s">
-        <v>169</v>
+        <v>164</v>
+      </c>
+      <c r="B50" s="88" t="s">
+        <v>168</v>
       </c>
       <c r="C50" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="100">
+      <c r="D50" s="95">
         <v>0.58333333333333337</v>
       </c>
       <c r="E50" s="77" t="s">
@@ -12178,7 +12174,7 @@
         <v>53</v>
       </c>
       <c r="BM50" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BN50" s="77" t="s">
         <v>53</v>
@@ -12189,15 +12185,15 @@
     </row>
     <row r="51" spans="1:67" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="77" t="s">
-        <v>166</v>
-      </c>
-      <c r="B51" s="94" t="s">
-        <v>170</v>
+        <v>165</v>
+      </c>
+      <c r="B51" s="89" t="s">
+        <v>169</v>
       </c>
       <c r="C51" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="D51" s="100">
+      <c r="D51" s="95">
         <v>0.41666666666666669</v>
       </c>
       <c r="E51" s="77" t="s">
@@ -12379,13 +12375,13 @@
         <v>56</v>
       </c>
       <c r="BK51" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BL51" s="86" t="s">
         <v>53</v>
       </c>
       <c r="BM51" s="77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BN51" s="77" t="s">
         <v>53</v>

</xml_diff>